<commit_message>
[Silverfox] Bad Cleaner 애니메이션 수정
</commit_message>
<xml_diff>
--- a/DesignDocs/VariableData/NPCTubeEnhancer.xlsx
+++ b/DesignDocs/VariableData/NPCTubeEnhancer.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\VariableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15430E81-9F17-4BF5-8B9A-AF5192CAE13C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="8112"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -336,7 +337,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -741,23 +742,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69921875" customWidth="1"/>
-    <col min="6" max="6" width="17.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" customWidth="1"/>
+    <col min="6" max="6" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -783,7 +784,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6100</v>
       </c>
@@ -809,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6101</v>
       </c>
@@ -835,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6102</v>
       </c>
@@ -861,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6103</v>
       </c>
@@ -887,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6104</v>
       </c>
@@ -913,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6105</v>
       </c>
@@ -939,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6106</v>
       </c>
@@ -965,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6107</v>
       </c>
@@ -985,13 +986,13 @@
         <v>11</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6108</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>6109</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>6110</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>6111</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>6112</v>
       </c>
@@ -1121,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>6113</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>6114</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>6115</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>6116</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>6117</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>6118</v>
       </c>
@@ -1277,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>6119</v>
       </c>
@@ -1303,7 +1304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>6120</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>6121</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>6122</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>6123</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>6124</v>
       </c>
@@ -1433,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>6125</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>6126</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>6127</v>
       </c>
@@ -1511,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>6128</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>6129</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>6130</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>6131</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>6132</v>
       </c>
@@ -1641,7 +1642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>6133</v>
       </c>
@@ -1667,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>6134</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>6135</v>
       </c>
@@ -1720,7 +1721,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>